<commit_message>
Add and modified Statistics
</commit_message>
<xml_diff>
--- a/statistic_sprungsweite_1.xlsx
+++ b/statistic_sprungsweite_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Semester\Unterlagen\Sicherer Programmierung\chess_server_strong - Kopie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Semester\Unterlagen\Sicherer Programmierung\chess_server_strong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26331C5E-8E42-487F-8A0F-922F3C936126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8541FC00-4B7C-47D8-A357-ACE86D734AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,154 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
-  <si>
-    <t>1 Spieler</t>
-  </si>
-  <si>
-    <t>2 Spieler</t>
-  </si>
-  <si>
-    <t>3 Spieler</t>
-  </si>
-  <si>
-    <t>4 Spieler</t>
-  </si>
-  <si>
-    <t>5 Spieler</t>
-  </si>
-  <si>
-    <t>6 Spieler</t>
-  </si>
-  <si>
-    <t>7 Spieler</t>
-  </si>
-  <si>
-    <t>8 Spieler</t>
-  </si>
-  <si>
-    <t>9 Spieler</t>
-  </si>
-  <si>
-    <t>10 Spieler</t>
-  </si>
-  <si>
-    <t>11 Spieler</t>
-  </si>
-  <si>
-    <t>12 Spieler</t>
-  </si>
-  <si>
-    <t>13 Spieler</t>
-  </si>
-  <si>
-    <t>14 Spieler</t>
-  </si>
-  <si>
-    <t>15 Spieler</t>
-  </si>
-  <si>
-    <t>16 Spieler</t>
-  </si>
-  <si>
-    <t>17 Spieler</t>
-  </si>
-  <si>
-    <t>18 Spieler</t>
-  </si>
-  <si>
-    <t>19 Spieler</t>
-  </si>
-  <si>
-    <t>20 Spieler</t>
-  </si>
-  <si>
-    <t>21 Spieler</t>
-  </si>
-  <si>
-    <t>22 Spieler</t>
-  </si>
-  <si>
-    <t>23 Spieler</t>
-  </si>
-  <si>
-    <t>24 Spieler</t>
-  </si>
-  <si>
-    <t>25 Spieler</t>
-  </si>
-  <si>
-    <t>26 Spieler</t>
-  </si>
-  <si>
-    <t>27 Spieler</t>
-  </si>
-  <si>
-    <t>28 Spieler</t>
-  </si>
-  <si>
-    <t>29 Spieler</t>
-  </si>
-  <si>
-    <t>30 Spieler</t>
-  </si>
-  <si>
-    <t>31 Spieler</t>
-  </si>
-  <si>
-    <t>32 Spieler</t>
-  </si>
-  <si>
-    <t>33 Spieler</t>
-  </si>
-  <si>
-    <t>34 Spieler</t>
-  </si>
-  <si>
-    <t>35 Spieler</t>
-  </si>
-  <si>
-    <t>36 Spieler</t>
-  </si>
-  <si>
-    <t>37 Spieler</t>
-  </si>
-  <si>
-    <t>38 Spieler</t>
-  </si>
-  <si>
-    <t>39 Spieler</t>
-  </si>
-  <si>
-    <t>40 Spieler</t>
-  </si>
-  <si>
-    <t>41 Spieler</t>
-  </si>
-  <si>
-    <t>42 Spieler</t>
-  </si>
-  <si>
-    <t>43 Spieler</t>
-  </si>
-  <si>
-    <t>44 Spieler</t>
-  </si>
-  <si>
-    <t>45 Spieler</t>
-  </si>
-  <si>
-    <t>46 Spieler</t>
-  </si>
-  <si>
-    <t>47 Spieler</t>
-  </si>
-  <si>
-    <t>48 Spieler</t>
-  </si>
-  <si>
-    <t>49 Spieler</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>CPU Auslastung</t>
   </si>
@@ -822,159 +675,160 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>statistic!$B$1:$AX$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>1 Spieler</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 Spieler</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3 Spieler</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4 Spieler</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5 Spieler</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6 Spieler</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7 Spieler</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8 Spieler</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9 Spieler</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10 Spieler</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11 Spieler</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12 Spieler</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13 Spieler</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14 Spieler</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15 Spieler</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16 Spieler</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17 Spieler</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18 Spieler</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19 Spieler</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20 Spieler</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21 Spieler</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22 Spieler</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23 Spieler</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24 Spieler</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25 Spieler</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26 Spieler</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27 Spieler</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28 Spieler</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29 Spieler</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30 Spieler</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31 Spieler</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32 Spieler</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>33 Spieler</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>34 Spieler</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>35 Spieler</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>36 Spieler</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37 Spieler</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38 Spieler</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>39 Spieler</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>40 Spieler</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41 Spieler</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42 Spieler</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>43 Spieler</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>44 Spieler</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>45 Spieler</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>46 Spieler</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>47 Spieler</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>48 Spieler</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>49 Spieler</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1181,159 +1035,160 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>statistic!$B$1:$AX$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>1 Spieler</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 Spieler</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3 Spieler</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4 Spieler</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5 Spieler</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6 Spieler</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7 Spieler</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8 Spieler</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9 Spieler</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10 Spieler</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11 Spieler</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12 Spieler</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13 Spieler</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14 Spieler</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15 Spieler</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16 Spieler</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17 Spieler</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18 Spieler</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19 Spieler</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20 Spieler</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21 Spieler</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22 Spieler</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23 Spieler</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24 Spieler</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25 Spieler</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26 Spieler</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27 Spieler</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28 Spieler</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29 Spieler</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30 Spieler</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31 Spieler</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32 Spieler</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>33 Spieler</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>34 Spieler</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>35 Spieler</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>36 Spieler</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37 Spieler</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38 Spieler</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>39 Spieler</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>40 Spieler</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41 Spieler</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42 Spieler</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>43 Spieler</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>44 Spieler</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>45 Spieler</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>46 Spieler</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>47 Spieler</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>48 Spieler</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>49 Spieler</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1518,6 +1373,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Spieler</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1701,7 +1611,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>CPU Auslastung in %</a:t>
+                  <a:t>CPU Auslastung</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2755,7 +2665,7 @@
   <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,157 +2674,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="K1">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M1">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N1">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="O1">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Q1">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="R1">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="S1">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="T1">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="U1">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="V1">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="W1">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="X1">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Y1">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="Z1">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AA1">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AB1">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AC1">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AD1">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AE1">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AF1">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AG1">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AH1">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AI1">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AJ1">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AK1">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AL1">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AM1">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AN1">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AO1">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AP1">
         <v>41</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AQ1">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AR1">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AS1">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AT1">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AU1">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AV1">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AW1">
         <v>48</v>
+      </c>
+      <c r="AX1">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>5.3604641437530498</v>
@@ -3066,7 +2976,7 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>41.32</v>

</xml_diff>